<commit_message>
updated shape file monthly data
</commit_message>
<xml_diff>
--- a/processed data/monthlycases.xlsx
+++ b/processed data/monthlycases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mygithub\data-indonesia-covid19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mygithub\data-indonesia-covid19\processed data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16803B6A-AE32-425C-A5C2-DCB9105D1BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44BA284-F26C-4789-BD96-972B105CC467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CD175747-2B29-40EF-9E3F-9AD965713BE2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -150,43 +150,97 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>casemar</t>
+    <t>case_mar</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>caseapr</t>
+    <t>case_apr</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>casemay</t>
+    <t>case_may</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>casejun</t>
+    <t>case_jun</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>casejul</t>
+    <t>case_jul</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>rateapr</t>
+    <t>case_chg</t>
+  </si>
+  <si>
+    <t>rate_mar</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ratemar</t>
+    <t>rate_apr</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ratemay</t>
+    <t>rate_may</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ratejun</t>
+    <t>rate_jun</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ratejul</t>
+    <t>rate_jul</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rate_chg</t>
+  </si>
+  <si>
+    <t>job_loss</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unemp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_retail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_groc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_parks</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_trans</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_work</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mob_all</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>THS_share_gdp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gdp_q1_yoy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gdp_q2_yoy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gdp_q2_qtq</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -236,7 +290,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -246,6 +300,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FABD15F-42DB-4ADF-BA5D-D61C82973FE3}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -571,13 +629,22 @@
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.25" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="8.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.58203125" customWidth="1"/>
-    <col min="9" max="11" width="8.08203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.08203125" customWidth="1"/>
-    <col min="13" max="13" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.58203125" customWidth="1"/>
+    <col min="10" max="12" width="8.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.08203125" customWidth="1"/>
+    <col min="15" max="15" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="18" max="18" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,25 +667,67 @@
         <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>1</v>
       </c>
@@ -646,31 +755,73 @@
         <v>415</v>
       </c>
       <c r="H2">
+        <v>75</v>
+      </c>
+      <c r="I2">
         <f>Sheet1!C38</f>
         <v>9.1576768805289477E-2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>Sheet1!D38</f>
         <v>0.18315353761057895</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>Sheet1!E38</f>
         <v>0.36630707522115791</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>Sheet1!F38</f>
         <v>1.4652283008846316</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>Sheet1!G38</f>
         <v>7.6008718108390267</v>
       </c>
-      <c r="M2">
+      <c r="N2">
+        <v>1.3736515320793421</v>
+      </c>
+      <c r="O2">
         <f>Sheet1!I2</f>
         <v>54.598999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="P2">
+        <v>15658</v>
+      </c>
+      <c r="Q2">
+        <v>5.42</v>
+      </c>
+      <c r="R2" s="3">
+        <v>-16.197802197802197</v>
+      </c>
+      <c r="S2" s="3">
+        <v>-2.9450549450549453</v>
+      </c>
+      <c r="T2" s="3">
+        <v>-16.703296703296704</v>
+      </c>
+      <c r="U2" s="3">
+        <v>-43.219780219780219</v>
+      </c>
+      <c r="V2" s="3">
+        <v>-18.736263736263737</v>
+      </c>
+      <c r="W2" s="3">
+        <v>-19.560439560439562</v>
+      </c>
+      <c r="X2">
+        <v>2.2886907110725279</v>
+      </c>
+      <c r="Y2">
+        <v>3.17</v>
+      </c>
+      <c r="Z2">
+        <v>-1.82</v>
+      </c>
+      <c r="AA2">
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>2</v>
       </c>
@@ -698,31 +849,73 @@
         <v>3407</v>
       </c>
       <c r="H3">
+        <v>1474</v>
+      </c>
+      <c r="I3">
         <f>Sheet1!C39</f>
         <v>0.4337107377647918</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>Sheet1!D39</f>
         <v>5.0675675675675675</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>Sheet1!E39</f>
         <v>10.614499634769905</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>Sheet1!F39</f>
         <v>34.080533235938638</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>Sheet1!G39</f>
         <v>77.771183345507666</v>
       </c>
-      <c r="M3">
+      <c r="N3">
+        <v>33.646822498173847</v>
+      </c>
+      <c r="O3">
         <f>Sheet1!I3</f>
         <v>43.808</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3">
+        <v>97105</v>
+      </c>
+      <c r="Q3">
+        <v>1.21</v>
+      </c>
+      <c r="R3" s="3">
+        <v>-44</v>
+      </c>
+      <c r="S3" s="3">
+        <v>-33.560439560439562</v>
+      </c>
+      <c r="T3" s="3">
+        <v>-59.516483516483518</v>
+      </c>
+      <c r="U3" s="3">
+        <v>-75.307692307692307</v>
+      </c>
+      <c r="V3" s="3">
+        <v>-38.857142857142854</v>
+      </c>
+      <c r="W3" s="3">
+        <v>-50.248351648351658</v>
+      </c>
+      <c r="X3">
+        <v>30.219639496708801</v>
+      </c>
+      <c r="Y3">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="Z3">
+        <v>-10.98</v>
+      </c>
+      <c r="AA3">
+        <v>-7.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>3</v>
       </c>
@@ -750,31 +943,73 @@
         <v>193</v>
       </c>
       <c r="H4">
+        <v>150</v>
+      </c>
+      <c r="I4">
         <f>Sheet1!C40</f>
         <v>0.13178703215603585</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>Sheet1!D40</f>
         <v>0.65893516078017922</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f>Sheet1!E40</f>
         <v>3.0311017395888245</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>Sheet1!F40</f>
         <v>10.015814443858725</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>Sheet1!G40</f>
         <v>12.717448603057459</v>
       </c>
-      <c r="M4">
+      <c r="N4">
+        <v>9.8840274117026894</v>
+      </c>
+      <c r="O4">
         <f>Sheet1!I4</f>
         <v>15.176</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="P4">
+        <v>18803</v>
+      </c>
+      <c r="Q4">
+        <v>3.41</v>
+      </c>
+      <c r="R4" s="3">
+        <v>-30.340659340659339</v>
+      </c>
+      <c r="S4" s="3">
+        <v>-7.813186813186813</v>
+      </c>
+      <c r="T4" s="3">
+        <v>-24.64835164835165</v>
+      </c>
+      <c r="U4" s="3">
+        <v>-63.989010989010985</v>
+      </c>
+      <c r="V4" s="3">
+        <v>-22.285714285714285</v>
+      </c>
+      <c r="W4" s="3">
+        <v>-29.815384615384612</v>
+      </c>
+      <c r="X4">
+        <v>8.1665409904746689</v>
+      </c>
+      <c r="Y4">
+        <v>1.35</v>
+      </c>
+      <c r="Z4">
+        <v>-4.9800000000000004</v>
+      </c>
+      <c r="AA4">
+        <v>-2.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>4</v>
       </c>
@@ -802,31 +1037,73 @@
         <v>1835</v>
       </c>
       <c r="H5">
+        <v>1311</v>
+      </c>
+      <c r="I5">
         <f>Sheet1!C41</f>
         <v>1.0789863607005814</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f>Sheet1!D41</f>
         <v>3.069792181148133</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f>Sheet1!E41</f>
         <v>6.5423046236845108</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f>Sheet1!F41</f>
         <v>11.04061395843623</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>Sheet1!G41</f>
         <v>13.943239238630753</v>
       </c>
-      <c r="M5">
+      <c r="N5">
+        <v>9.9616275977356494</v>
+      </c>
+      <c r="O5">
         <f>Sheet1!I5</f>
         <v>131.60499999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="P5">
+        <v>67736</v>
+      </c>
+      <c r="Q5">
+        <v>8.01</v>
+      </c>
+      <c r="R5" s="3">
+        <v>-31.032967032967033</v>
+      </c>
+      <c r="S5" s="3">
+        <v>-12.428571428571429</v>
+      </c>
+      <c r="T5" s="3">
+        <v>-20.285714285714285</v>
+      </c>
+      <c r="U5" s="3">
+        <v>-61.989010989010985</v>
+      </c>
+      <c r="V5" s="3">
+        <v>-31.901098901098901</v>
+      </c>
+      <c r="W5" s="3">
+        <v>-31.527472527472526</v>
+      </c>
+      <c r="X5">
+        <v>11.572395719589428</v>
+      </c>
+      <c r="Y5">
+        <v>3.19</v>
+      </c>
+      <c r="Z5">
+        <v>-7.4</v>
+      </c>
+      <c r="AA5">
+        <v>-8.5500000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>5</v>
       </c>
@@ -854,31 +1131,73 @@
         <v>217</v>
       </c>
       <c r="H6">
+        <v>124</v>
+      </c>
+      <c r="I6">
         <f>Sheet1!C42</f>
         <v>4.9509852460639665E-2</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>Sheet1!D42</f>
         <v>0.59411822952767601</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>Sheet1!E42</f>
         <v>4.50539657391821</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>Sheet1!F42</f>
         <v>6.188731557579958</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>Sheet1!G42</f>
         <v>10.743637983958807</v>
       </c>
-      <c r="M6">
+      <c r="N6">
+        <v>6.1392217051193185</v>
+      </c>
+      <c r="O6">
         <f>Sheet1!I6</f>
         <v>20.198</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="P6">
+        <v>7603</v>
+      </c>
+      <c r="Q6">
+        <v>3.22</v>
+      </c>
+      <c r="R6" s="3">
+        <v>-22.065934065934066</v>
+      </c>
+      <c r="S6" s="3">
+        <v>-9.4065934065934069</v>
+      </c>
+      <c r="T6" s="3">
+        <v>-27.164835164835164</v>
+      </c>
+      <c r="U6" s="3">
+        <v>-52.879120879120876</v>
+      </c>
+      <c r="V6" s="3">
+        <v>-23.35164835164835</v>
+      </c>
+      <c r="W6" s="3">
+        <v>-26.97362637362637</v>
+      </c>
+      <c r="X6">
+        <v>13.031912697455718</v>
+      </c>
+      <c r="Y6">
+        <v>3.8</v>
+      </c>
+      <c r="Z6">
+        <v>-0.48</v>
+      </c>
+      <c r="AA6">
+        <v>-2.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>6</v>
       </c>
@@ -906,31 +1225,73 @@
         <v>1015</v>
       </c>
       <c r="H7">
+        <v>249</v>
+      </c>
+      <c r="I7">
         <f>Sheet1!C43</f>
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>Sheet1!D43</f>
         <v>1.2299114463758609</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>Sheet1!E43</f>
         <v>7.7074450639553955</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>Sheet1!F43</f>
         <v>20.416530009839292</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>Sheet1!G43</f>
         <v>83.224007871433258</v>
       </c>
-      <c r="M7">
+      <c r="N7">
+        <v>20.416530009839292</v>
+      </c>
+      <c r="O7">
         <f>Sheet1!I7</f>
         <v>12.196</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="P7">
+        <v>10201</v>
+      </c>
+      <c r="Q7">
+        <v>3.59</v>
+      </c>
+      <c r="R7" s="3">
+        <v>-30.219780219780219</v>
+      </c>
+      <c r="S7" s="3">
+        <v>-16.912087912087912</v>
+      </c>
+      <c r="T7" s="3">
+        <v>-13.406593406593407</v>
+      </c>
+      <c r="U7" s="3">
+        <v>-45.684210526315788</v>
+      </c>
+      <c r="V7" s="3">
+        <v>-26.098901098901099</v>
+      </c>
+      <c r="W7" s="3">
+        <v>-26.464314632735686</v>
+      </c>
+      <c r="X7">
+        <v>9.7732342085882333</v>
+      </c>
+      <c r="Y7">
+        <v>4.05</v>
+      </c>
+      <c r="Z7">
+        <v>-0.27</v>
+      </c>
+      <c r="AA7">
+        <v>-3.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>7</v>
       </c>
@@ -958,31 +1319,73 @@
         <v>433</v>
       </c>
       <c r="H8">
+        <v>237</v>
+      </c>
+      <c r="I8">
         <f>Sheet1!C44</f>
         <v>0.20370747606437156</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>Sheet1!D44</f>
         <v>3.7685883071908739</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f>Sheet1!E44</f>
         <v>17.111427989407211</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f>Sheet1!F44</f>
         <v>24.343043389692404</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>Sheet1!G44</f>
         <v>44.102668567936448</v>
       </c>
-      <c r="M8">
+      <c r="N8">
+        <v>24.139335913628031</v>
+      </c>
+      <c r="O8">
         <f>Sheet1!I8</f>
         <v>9.8179999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="P8">
+        <v>7848</v>
+      </c>
+      <c r="Q8">
+        <v>6.2</v>
+      </c>
+      <c r="R8" s="3">
+        <v>-30.582417582417584</v>
+      </c>
+      <c r="S8" s="3">
+        <v>-16.318681318681318</v>
+      </c>
+      <c r="T8" s="3">
+        <v>-34.934065934065934</v>
+      </c>
+      <c r="U8" s="3">
+        <v>-61.912087912087912</v>
+      </c>
+      <c r="V8" s="3">
+        <v>-23.87912087912088</v>
+      </c>
+      <c r="W8" s="3">
+        <v>-33.525274725274727</v>
+      </c>
+      <c r="X8">
+        <v>3.6873746203362798</v>
+      </c>
+      <c r="Y8">
+        <v>5.14</v>
+      </c>
+      <c r="Z8">
+        <v>0.53</v>
+      </c>
+      <c r="AA8">
+        <v>-2.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1010,31 +1413,73 @@
         <v>21399</v>
       </c>
       <c r="H9">
+        <v>10677</v>
+      </c>
+      <c r="I9">
         <f>Sheet1!C45</f>
         <v>7.0173790511977456</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f>Sheet1!D45</f>
         <v>39.220291216533582</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f>Sheet1!E45</f>
         <v>69.027712541099106</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f>Sheet1!F45</f>
         <v>107.3179896665101</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>Sheet1!G45</f>
         <v>201.02395490840769</v>
       </c>
-      <c r="M9">
+      <c r="N9">
+        <v>100.30061061531235</v>
+      </c>
+      <c r="O9">
         <f>Sheet1!I9</f>
         <v>106.45</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="P9">
+        <v>320114</v>
+      </c>
+      <c r="Q9">
+        <v>4.93</v>
+      </c>
+      <c r="R9" s="3">
+        <v>-27</v>
+      </c>
+      <c r="S9" s="3">
+        <v>-3</v>
+      </c>
+      <c r="T9" s="3">
+        <v>-77</v>
+      </c>
+      <c r="U9" s="3">
+        <v>-45</v>
+      </c>
+      <c r="V9" s="3">
+        <v>-33</v>
+      </c>
+      <c r="W9" s="3">
+        <v>-37</v>
+      </c>
+      <c r="X9">
+        <v>20.972147115654213</v>
+      </c>
+      <c r="Y9">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="Z9">
+        <v>-8.2200000000000006</v>
+      </c>
+      <c r="AA9">
+        <v>-11.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1062,31 +1507,73 @@
         <v>162</v>
       </c>
       <c r="H10">
+        <v>115</v>
+      </c>
+      <c r="I10">
         <f>Sheet1!C46</f>
         <v>5.4378857500203916E-2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f>Sheet1!D46</f>
         <v>0.87006172000326265</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f>Sheet1!E46</f>
         <v>2.6373745887598901</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f>Sheet1!F46</f>
         <v>3.1811631637619291</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f>Sheet1!G46</f>
         <v>4.4046874575165171</v>
       </c>
-      <c r="M10">
+      <c r="N10">
+        <v>3.1267843062617251</v>
+      </c>
+      <c r="O10">
         <f>Sheet1!I10</f>
         <v>36.779000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="P10">
+        <v>16900</v>
+      </c>
+      <c r="Q10">
+        <v>4.41</v>
+      </c>
+      <c r="R10" s="3">
+        <v>-10</v>
+      </c>
+      <c r="S10" s="3">
+        <v>3</v>
+      </c>
+      <c r="T10" s="3">
+        <v>-7</v>
+      </c>
+      <c r="U10" s="3">
+        <v>-27</v>
+      </c>
+      <c r="V10" s="3">
+        <v>-17</v>
+      </c>
+      <c r="W10" s="3">
+        <v>-11.6</v>
+      </c>
+      <c r="X10">
+        <v>6.4869964822873962</v>
+      </c>
+      <c r="Y10">
+        <v>1.87</v>
+      </c>
+      <c r="Z10">
+        <v>-1.72</v>
+      </c>
+      <c r="AA10">
+        <v>-1.41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1114,31 +1601,73 @@
         <v>6532</v>
       </c>
       <c r="H11">
+        <v>3020</v>
+      </c>
+      <c r="I11">
         <f>Sheet1!C47</f>
         <v>0.39650991174650596</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>Sheet1!D47</f>
         <v>2.0266062155932527</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f>Sheet1!E47</f>
         <v>4.5258202047833516</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f>Sheet1!F47</f>
         <v>6.4442873535366481</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f>Sheet1!G47</f>
         <v>13.080821937010995</v>
       </c>
-      <c r="M11">
+      <c r="N11">
+        <v>6.0477774417901422</v>
+      </c>
+      <c r="O11">
         <f>Sheet1!I11</f>
         <v>499.35700000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="P11">
+        <v>342772</v>
+      </c>
+      <c r="Q11">
+        <v>7.69</v>
+      </c>
+      <c r="R11" s="3">
+        <v>-23</v>
+      </c>
+      <c r="S11" s="3">
+        <v>9</v>
+      </c>
+      <c r="T11" s="3">
+        <v>-2</v>
+      </c>
+      <c r="U11" s="3">
+        <v>-29</v>
+      </c>
+      <c r="V11" s="3">
+        <v>-25</v>
+      </c>
+      <c r="W11" s="3">
+        <v>-14</v>
+      </c>
+      <c r="X11">
+        <v>10.171990830730458</v>
+      </c>
+      <c r="Y11">
+        <v>2.73</v>
+      </c>
+      <c r="Z11">
+        <v>-5.98</v>
+      </c>
+      <c r="AA11">
+        <v>-4.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1166,31 +1695,73 @@
         <v>9516</v>
       </c>
       <c r="H12">
+        <v>3740</v>
+      </c>
+      <c r="I12">
         <f>Sheet1!C48</f>
         <v>0.26616981634282671</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f>Sheet1!D48</f>
         <v>2.0721177100237265</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f>Sheet1!E48</f>
         <v>4.0154435734299554</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f>Sheet1!F48</f>
         <v>10.970203290774784</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f>Sheet1!G48</f>
         <v>27.235182498046655</v>
       </c>
-      <c r="M12">
+      <c r="N12">
+        <v>10.704033474431958</v>
+      </c>
+      <c r="O12">
         <f>Sheet1!I12</f>
         <v>349.40100000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="P12">
+        <v>263980</v>
+      </c>
+      <c r="Q12">
+        <v>4.25</v>
+      </c>
+      <c r="R12">
+        <v>-6</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>-9</v>
+      </c>
+      <c r="U12">
+        <v>-34</v>
+      </c>
+      <c r="V12">
+        <v>-20</v>
+      </c>
+      <c r="W12" s="3">
+        <v>-13.4</v>
+      </c>
+      <c r="X12">
+        <v>9.0397164957138862</v>
+      </c>
+      <c r="Y12">
+        <v>2.61</v>
+      </c>
+      <c r="Z12">
+        <v>-5.94</v>
+      </c>
+      <c r="AA12">
+        <v>-5.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1218,31 +1789,73 @@
         <v>22089</v>
       </c>
       <c r="H13">
+        <v>12043</v>
+      </c>
+      <c r="I13">
         <f>Sheet1!C49</f>
         <v>0.2331627651599672</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f>Sheet1!D49</f>
         <v>2.401827193798372</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f>Sheet1!E49</f>
         <v>12.17711344496732</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f>Sheet1!F49</f>
         <v>30.426487290122171</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f>Sheet1!G49</f>
         <v>55.379917415252855</v>
       </c>
-      <c r="M13">
+      <c r="N13">
+        <v>30.193324524962204</v>
+      </c>
+      <c r="O13">
         <f>Sheet1!I13</f>
         <v>398.863</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="P13">
+        <v>161217</v>
+      </c>
+      <c r="Q13">
+        <v>3.69</v>
+      </c>
+      <c r="R13">
+        <v>-11</v>
+      </c>
+      <c r="S13">
+        <v>-1</v>
+      </c>
+      <c r="T13">
+        <v>-14</v>
+      </c>
+      <c r="U13">
+        <v>-37</v>
+      </c>
+      <c r="V13">
+        <v>-23</v>
+      </c>
+      <c r="W13" s="3">
+        <v>-17.2</v>
+      </c>
+      <c r="X13">
+        <v>10.726832364448653</v>
+      </c>
+      <c r="Y13">
+        <v>3.02</v>
+      </c>
+      <c r="Z13">
+        <v>-5.9</v>
+      </c>
+      <c r="AA13">
+        <v>-5.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1270,31 +1883,73 @@
         <v>387</v>
       </c>
       <c r="H14">
+        <v>312</v>
+      </c>
+      <c r="I14">
         <f>Sheet1!C50</f>
         <v>0.1752745968684272</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f>Sheet1!D50</f>
         <v>1.1295474020409753</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f>Sheet1!E50</f>
         <v>3.6807665342369713</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f>Sheet1!F50</f>
         <v>6.2514606216405699</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f>Sheet1!G50</f>
         <v>7.5368076653423701</v>
       </c>
-      <c r="M14">
+      <c r="N14">
+        <v>6.0761860247721424</v>
+      </c>
+      <c r="O14">
         <f>Sheet1!I14</f>
         <v>51.347999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="P14">
+        <v>18645</v>
+      </c>
+      <c r="Q14">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="R14">
+        <v>-19</v>
+      </c>
+      <c r="S14">
+        <v>-6</v>
+      </c>
+      <c r="T14">
+        <v>-11</v>
+      </c>
+      <c r="U14">
+        <v>-36</v>
+      </c>
+      <c r="V14">
+        <v>-20</v>
+      </c>
+      <c r="W14" s="3">
+        <v>-18.399999999999999</v>
+      </c>
+      <c r="X14">
+        <v>8.1691805691351131</v>
+      </c>
+      <c r="Y14">
+        <v>2.69</v>
+      </c>
+      <c r="Z14">
+        <v>-3.4</v>
+      </c>
+      <c r="AA14">
+        <v>-8.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1322,31 +1977,73 @@
         <v>6098</v>
       </c>
       <c r="H15">
+        <v>3140</v>
+      </c>
+      <c r="I15">
         <f>Sheet1!C51</f>
         <v>0.18587360594795541</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f>Sheet1!D51</f>
         <v>3.949814126394052</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f>Sheet1!E51</f>
         <v>21.352230483271377</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <f>Sheet1!F51</f>
         <v>73.141263940520446</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f>Sheet1!G51</f>
         <v>141.68215613382901</v>
       </c>
-      <c r="M15">
+      <c r="N15">
+        <v>72.955390334572485</v>
+      </c>
+      <c r="O15">
         <f>Sheet1!I15</f>
         <v>43.04</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="P15">
+        <v>27994</v>
+      </c>
+      <c r="Q15">
+        <v>3.8</v>
+      </c>
+      <c r="R15">
+        <v>-16</v>
+      </c>
+      <c r="S15">
+        <v>-8</v>
+      </c>
+      <c r="T15">
+        <v>-19</v>
+      </c>
+      <c r="U15">
+        <v>-38</v>
+      </c>
+      <c r="V15">
+        <v>-23</v>
+      </c>
+      <c r="W15" s="3">
+        <v>-20.8</v>
+      </c>
+      <c r="X15">
+        <v>9.9414362909659104</v>
+      </c>
+      <c r="Y15">
+        <v>4.18</v>
+      </c>
+      <c r="Z15">
+        <v>-2.61</v>
+      </c>
+      <c r="AA15">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1374,31 +2071,73 @@
         <v>1729</v>
       </c>
       <c r="H16">
+        <v>885</v>
+      </c>
+      <c r="I16">
         <f>Sheet1!C52</f>
         <v>0.32500361115123499</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f>Sheet1!D52</f>
         <v>5.2361692907698973</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f>Sheet1!E52</f>
         <v>14.805720063556262</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <f>Sheet1!F52</f>
         <v>32.283692041022675</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f>Sheet1!G52</f>
         <v>62.436804853387258</v>
       </c>
-      <c r="M16">
+      <c r="N16">
+        <v>31.95868842987144</v>
+      </c>
+      <c r="O16">
         <f>Sheet1!I16</f>
         <v>27.692</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="P16">
+        <v>12371</v>
+      </c>
+      <c r="Q16">
+        <v>3.39</v>
+      </c>
+      <c r="R16">
+        <v>-17</v>
+      </c>
+      <c r="S16">
+        <v>-9</v>
+      </c>
+      <c r="T16">
+        <v>-20</v>
+      </c>
+      <c r="U16">
+        <v>-23</v>
+      </c>
+      <c r="V16">
+        <v>-17</v>
+      </c>
+      <c r="W16" s="3">
+        <v>-17.2</v>
+      </c>
+      <c r="X16">
+        <v>9.2255592530414638</v>
+      </c>
+      <c r="Y16">
+        <v>2.95</v>
+      </c>
+      <c r="Z16">
+        <v>-3.15</v>
+      </c>
+      <c r="AA16">
+        <v>-5.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1426,31 +2165,73 @@
         <v>1426</v>
       </c>
       <c r="H17">
+        <v>498</v>
+      </c>
+      <c r="I17">
         <f>Sheet1!C53</f>
         <v>0.52718981469278015</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f>Sheet1!D53</f>
         <v>3.5321717584416272</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f>Sheet1!E53</f>
         <v>7.7760497667185078</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <f>Sheet1!F53</f>
         <v>13.654216200543006</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f>Sheet1!G53</f>
         <v>37.588633787595228</v>
       </c>
-      <c r="M17">
+      <c r="N17">
+        <v>13.127026385850225</v>
+      </c>
+      <c r="O17">
         <f>Sheet1!I17</f>
         <v>37.936999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="P17">
+        <v>46689</v>
+      </c>
+      <c r="Q17">
+        <v>6.88</v>
+      </c>
+      <c r="R17">
+        <v>-11</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="T17">
+        <v>-5</v>
+      </c>
+      <c r="U17">
+        <v>-34</v>
+      </c>
+      <c r="V17">
+        <v>-17</v>
+      </c>
+      <c r="W17" s="3">
+        <v>-12.8</v>
+      </c>
+      <c r="X17">
+        <v>4.5639687568988663</v>
+      </c>
+      <c r="Y17">
+        <v>1.27</v>
+      </c>
+      <c r="Z17">
+        <v>-5.46</v>
+      </c>
+      <c r="AA17">
+        <v>-6.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1478,31 +2259,73 @@
         <v>283</v>
       </c>
       <c r="H18">
+        <v>204</v>
+      </c>
+      <c r="I18">
         <f>Sheet1!C54</f>
         <v>0.26041666666666669</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f>Sheet1!D54</f>
         <v>13.020833333333334</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f>Sheet1!E54</f>
         <v>21.484375</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <f>Sheet1!F54</f>
         <v>26.822916666666668</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f>Sheet1!G54</f>
         <v>36.848958333333336</v>
       </c>
-      <c r="M18">
+      <c r="N18">
+        <v>26.5625</v>
+      </c>
+      <c r="O18">
         <f>Sheet1!I18</f>
         <v>7.68</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="P18">
+        <v>8721</v>
+      </c>
+      <c r="Q18">
+        <v>5.65</v>
+      </c>
+      <c r="R18">
+        <v>-13</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>-10</v>
+      </c>
+      <c r="U18">
+        <v>-25</v>
+      </c>
+      <c r="V18">
+        <v>-12</v>
+      </c>
+      <c r="W18" s="3">
+        <v>-11</v>
+      </c>
+      <c r="X18">
+        <v>8.7372333673388471</v>
+      </c>
+      <c r="Y18">
+        <v>5.01</v>
+      </c>
+      <c r="Z18">
+        <v>-3.35</v>
+      </c>
+      <c r="AA18">
+        <v>-6.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1530,31 +2353,73 @@
         <v>447</v>
       </c>
       <c r="H19">
+        <v>286</v>
+      </c>
+      <c r="I19">
         <f>Sheet1!C55</f>
         <v>0.31219338150031217</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f>Sheet1!D55</f>
         <v>3.9693158505039694</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f>Sheet1!E55</f>
         <v>8.7860137365087851</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <f>Sheet1!F55</f>
         <v>13.067522968513067</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f>Sheet1!G55</f>
         <v>19.935777361519936</v>
       </c>
-      <c r="M19">
+      <c r="N19">
+        <v>12.755329587012755</v>
+      </c>
+      <c r="O19">
         <f>Sheet1!I19</f>
         <v>22.422000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="P19">
+        <v>42102</v>
+      </c>
+      <c r="Q19">
+        <v>5.57</v>
+      </c>
+      <c r="R19">
+        <v>-16</v>
+      </c>
+      <c r="S19">
+        <v>-7</v>
+      </c>
+      <c r="T19">
+        <v>-14</v>
+      </c>
+      <c r="U19">
+        <v>-57</v>
+      </c>
+      <c r="V19">
+        <v>-16</v>
+      </c>
+      <c r="W19" s="3">
+        <v>-22</v>
+      </c>
+      <c r="X19">
+        <v>9.9853993028321035</v>
+      </c>
+      <c r="Y19">
+        <v>2.06</v>
+      </c>
+      <c r="Z19">
+        <v>-6.66</v>
+      </c>
+      <c r="AA19">
+        <v>-7.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1582,31 +2447,73 @@
         <v>255</v>
       </c>
       <c r="H20">
+        <v>182</v>
+      </c>
+      <c r="I20">
         <f>Sheet1!C56</f>
         <v>9.388349058818006E-2</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f>Sheet1!D56</f>
         <v>0.53983007088203538</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f>Sheet1!E56</f>
         <v>1.5608130310284936</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <f>Sheet1!F56</f>
         <v>2.2297329014692764</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f>Sheet1!G56</f>
         <v>2.9925362624982395</v>
       </c>
-      <c r="M20">
+      <c r="N20">
+        <v>2.1358494108810961</v>
+      </c>
+      <c r="O20">
         <f>Sheet1!I20</f>
         <v>85.212000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="P20">
+        <v>27571</v>
+      </c>
+      <c r="Q20">
+        <v>4.28</v>
+      </c>
+      <c r="R20">
+        <v>-6</v>
+      </c>
+      <c r="S20">
+        <v>8</v>
+      </c>
+      <c r="T20">
+        <v>-12</v>
+      </c>
+      <c r="U20">
+        <v>-30</v>
+      </c>
+      <c r="V20">
+        <v>-23</v>
+      </c>
+      <c r="W20" s="3">
+        <v>-12.6</v>
+      </c>
+      <c r="X20">
+        <v>7.8565402319458526</v>
+      </c>
+      <c r="Y20">
+        <v>1.74</v>
+      </c>
+      <c r="Z20">
+        <v>-3.57</v>
+      </c>
+      <c r="AA20">
+        <v>-0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1634,31 +2541,73 @@
         <v>1530</v>
       </c>
       <c r="H21">
+        <v>727</v>
+      </c>
+      <c r="I21">
         <f>Sheet1!C57</f>
         <v>7.8198310916484201E-2</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f>Sheet1!D57</f>
         <v>3.1279324366593682</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f>Sheet1!E57</f>
         <v>11.964341570222082</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <f>Sheet1!F57</f>
         <v>56.928370347200499</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f>Sheet1!G57</f>
         <v>119.64341570222084</v>
       </c>
-      <c r="M21">
+      <c r="N21">
+        <v>56.850172036284015</v>
+      </c>
+      <c r="O21">
         <f>Sheet1!I21</f>
         <v>12.788</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="P21">
+        <v>3567</v>
+      </c>
+      <c r="Q21">
+        <v>4.26</v>
+      </c>
+      <c r="R21">
+        <v>-22</v>
+      </c>
+      <c r="S21">
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>-20</v>
+      </c>
+      <c r="U21">
+        <v>-31</v>
+      </c>
+      <c r="V21">
+        <v>-15</v>
+      </c>
+      <c r="W21" s="3">
+        <v>-16.600000000000001</v>
+      </c>
+      <c r="X21">
+        <v>7.4434874186632571</v>
+      </c>
+      <c r="Y21">
+        <v>3.06</v>
+      </c>
+      <c r="Z21">
+        <v>-0.16</v>
+      </c>
+      <c r="AA21">
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1686,31 +2635,73 @@
         <v>1093</v>
       </c>
       <c r="H22">
+        <v>741</v>
+      </c>
+      <c r="I22">
         <f>Sheet1!C58</f>
         <v>5.4588132539985811E-2</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f>Sheet1!D58</f>
         <v>1.2555270484196737</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f>Sheet1!E58</f>
         <v>12.173153556416835</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <f>Sheet1!F58</f>
         <v>40.504394344669471</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f>Sheet1!G58</f>
         <v>59.664828866204488</v>
       </c>
-      <c r="M22">
+      <c r="N22">
+        <v>40.449806212129488</v>
+      </c>
+      <c r="O22">
         <f>Sheet1!I22</f>
         <v>18.318999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="P22">
+        <v>14365</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>7.02</v>
+      </c>
+      <c r="R22">
+        <v>-47</v>
+      </c>
+      <c r="S22">
+        <v>-38</v>
+      </c>
+      <c r="T22">
+        <v>-31</v>
+      </c>
+      <c r="U22">
+        <v>-57</v>
+      </c>
+      <c r="V22">
+        <v>-31</v>
+      </c>
+      <c r="W22" s="3">
+        <v>-40.799999999999997</v>
+      </c>
+      <c r="X22">
+        <v>14.107633440849199</v>
+      </c>
+      <c r="Y22">
+        <v>4</v>
+      </c>
+      <c r="Z22">
+        <v>-0.92</v>
+      </c>
+      <c r="AA22">
+        <v>-2.61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1738,31 +2729,73 @@
         <v>2065</v>
       </c>
       <c r="H23">
+        <v>1230</v>
+      </c>
+      <c r="I23">
         <f>Sheet1!C59</f>
         <v>7.8039644139222722E-2</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f>Sheet1!D59</f>
         <v>4.487279538005307</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f>Sheet1!E59</f>
         <v>12.408303418136413</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <f>Sheet1!F59</f>
         <v>24.07523021695021</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f>Sheet1!G59</f>
         <v>40.287966286873733</v>
       </c>
-      <c r="M23">
+      <c r="N23">
+        <v>23.997190572810986</v>
+      </c>
+      <c r="O23">
         <f>Sheet1!I23</f>
         <v>51.256</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="P23">
+        <v>48448</v>
+      </c>
+      <c r="Q23">
+        <v>3.14</v>
+      </c>
+      <c r="R23">
+        <v>-17</v>
+      </c>
+      <c r="S23">
+        <v>-6</v>
+      </c>
+      <c r="T23">
+        <v>-18</v>
+      </c>
+      <c r="U23">
+        <v>-53</v>
+      </c>
+      <c r="V23">
+        <v>-19</v>
+      </c>
+      <c r="W23" s="3">
+        <v>-22.6</v>
+      </c>
+      <c r="X23">
+        <v>11.293103005929177</v>
+      </c>
+      <c r="Y23">
+        <v>3.02</v>
+      </c>
+      <c r="Z23">
+        <v>-1.41</v>
+      </c>
+      <c r="AA23">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1790,31 +2823,73 @@
         <v>145</v>
       </c>
       <c r="H24">
+        <v>113</v>
+      </c>
+      <c r="I24">
         <f>Sheet1!C60</f>
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f>Sheet1!D60</f>
         <v>5.4137943479987002E-2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f>Sheet1!E60</f>
         <v>1.6602302667196016</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <f>Sheet1!F60</f>
         <v>2.0391958710795106</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f>Sheet1!G60</f>
         <v>2.6166672681993721</v>
       </c>
-      <c r="M24">
+      <c r="N24">
+        <v>2.0391958710795106</v>
+      </c>
+      <c r="O24">
         <f>Sheet1!I24</f>
         <v>55.414000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="P24">
+        <v>22865</v>
+      </c>
+      <c r="Q24">
+        <v>2.8</v>
+      </c>
+      <c r="R24">
+        <v>-11</v>
+      </c>
+      <c r="S24">
+        <v>-3</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>-27</v>
+      </c>
+      <c r="V24">
+        <v>-9</v>
+      </c>
+      <c r="W24" s="3">
+        <v>-10</v>
+      </c>
+      <c r="X24">
+        <v>8.4769904343151339</v>
+      </c>
+      <c r="Y24">
+        <v>2.98</v>
+      </c>
+      <c r="Z24">
+        <v>-1.96</v>
+      </c>
+      <c r="AA24">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1842,31 +2917,73 @@
         <v>3059</v>
       </c>
       <c r="H25">
+        <v>1740</v>
+      </c>
+      <c r="I25">
         <f>Sheet1!C61</f>
         <v>0.29108691855388019</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f>Sheet1!D61</f>
         <v>5.9672818303545441</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f>Sheet1!E61</f>
         <v>19.648367002386912</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <f>Sheet1!F61</f>
         <v>50.940210746929033</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f>Sheet1!G61</f>
         <v>89.043488385631946</v>
       </c>
-      <c r="M25">
+      <c r="N25">
+        <v>50.649123828375153</v>
+      </c>
+      <c r="O25">
         <f>Sheet1!I25</f>
         <v>34.353999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="P25">
+        <v>4525</v>
+      </c>
+      <c r="Q25">
+        <v>3.62</v>
+      </c>
+      <c r="R25">
+        <v>-24</v>
+      </c>
+      <c r="S25">
+        <v>-15</v>
+      </c>
+      <c r="T25">
+        <v>-17</v>
+      </c>
+      <c r="U25">
+        <v>-38</v>
+      </c>
+      <c r="V25">
+        <v>-15</v>
+      </c>
+      <c r="W25" s="3">
+        <v>-21.8</v>
+      </c>
+      <c r="X25">
+        <v>8.8943091681000794</v>
+      </c>
+      <c r="Y25">
+        <v>1.48</v>
+      </c>
+      <c r="Z25">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="AA25">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1894,31 +3011,73 @@
         <v>445</v>
       </c>
       <c r="H26">
+        <v>223</v>
+      </c>
+      <c r="I26">
         <f>Sheet1!C62</f>
         <v>4.2085770800892215E-2</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f>Sheet1!D62</f>
         <v>0.57517220094552701</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f>Sheet1!E62</f>
         <v>1.6413450612347964</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <f>Sheet1!F62</f>
         <v>3.1704614003338802</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f>Sheet1!G62</f>
         <v>6.2427226687990123</v>
       </c>
-      <c r="M26">
+      <c r="N26">
+        <v>3.1283756295329881</v>
+      </c>
+      <c r="O26">
         <f>Sheet1!I26</f>
         <v>71.283000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="P26">
+        <v>156146</v>
+      </c>
+      <c r="Q26">
+        <v>5.07</v>
+      </c>
+      <c r="R26">
+        <v>-9</v>
+      </c>
+      <c r="S26">
+        <v>-3</v>
+      </c>
+      <c r="T26">
+        <v>-7</v>
+      </c>
+      <c r="U26">
+        <v>-39</v>
+      </c>
+      <c r="V26">
+        <v>-17</v>
+      </c>
+      <c r="W26" s="3">
+        <v>-15</v>
+      </c>
+      <c r="X26">
+        <v>1.8860865579354273</v>
+      </c>
+      <c r="Y26">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Z26">
+        <v>-3.22</v>
+      </c>
+      <c r="AA26">
+        <v>-4.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1946,31 +3105,73 @@
         <v>230</v>
       </c>
       <c r="H27">
+        <v>114</v>
+      </c>
+      <c r="I27">
         <f>Sheet1!C63</f>
         <v>7.1174377224199281E-2</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f>Sheet1!D63</f>
         <v>2.9893238434163698</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f>Sheet1!E63</f>
         <v>6.5480427046263339</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <f>Sheet1!F63</f>
         <v>8.185053380782918</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f>Sheet1!G63</f>
         <v>16.370106761565836</v>
       </c>
-      <c r="M27">
+      <c r="N27">
+        <v>8.1138790035587185</v>
+      </c>
+      <c r="O27">
         <f>Sheet1!I27</f>
         <v>14.05</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="P27">
+        <v>6115</v>
+      </c>
+      <c r="Q27">
+        <v>2.61</v>
+      </c>
+      <c r="R27">
+        <v>-10</v>
+      </c>
+      <c r="S27">
+        <v>-3</v>
+      </c>
+      <c r="T27">
+        <v>-20</v>
+      </c>
+      <c r="U27">
+        <v>-42</v>
+      </c>
+      <c r="V27">
+        <v>-12</v>
+      </c>
+      <c r="W27" s="3">
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="X27">
+        <v>3.9614587474659002</v>
+      </c>
+      <c r="Y27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Z27">
+        <v>-0.78</v>
+      </c>
+      <c r="AA27">
+        <v>-1.27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1998,31 +3199,73 @@
         <v>9422</v>
       </c>
       <c r="H28">
+        <v>5034</v>
+      </c>
+      <c r="I28">
         <f>Sheet1!C64</f>
         <v>0.56003584229390679</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f>Sheet1!D64</f>
         <v>5.4995519713261647</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f>Sheet1!E64</f>
         <v>17.260304659498207</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <f>Sheet1!F64</f>
         <v>56.944444444444443</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f>Sheet1!G64</f>
         <v>105.5331541218638</v>
       </c>
-      <c r="M28">
+      <c r="N28">
+        <v>56.384408602150536</v>
+      </c>
+      <c r="O28">
         <f>Sheet1!I28</f>
         <v>89.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="P28">
+        <v>41908</v>
+      </c>
+      <c r="Q28">
+        <v>6.07</v>
+      </c>
+      <c r="R28">
+        <v>-20</v>
+      </c>
+      <c r="S28">
+        <v>-5</v>
+      </c>
+      <c r="T28">
+        <v>-10</v>
+      </c>
+      <c r="U28">
+        <v>-52</v>
+      </c>
+      <c r="V28">
+        <v>-26</v>
+      </c>
+      <c r="W28" s="3">
+        <v>-22.6</v>
+      </c>
+      <c r="X28">
+        <v>7.0043853016785116</v>
+      </c>
+      <c r="Y28">
+        <v>3.07</v>
+      </c>
+      <c r="Z28">
+        <v>-3.87</v>
+      </c>
+      <c r="AA28">
+        <v>-0.41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2050,31 +3293,73 @@
         <v>207</v>
       </c>
       <c r="H29">
+        <v>186</v>
+      </c>
+      <c r="I29">
         <f>Sheet1!C65</f>
         <v>9.6867936712948022E-2</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f>Sheet1!D65</f>
         <v>1.517597675169519</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <f>Sheet1!E65</f>
         <v>4.1330319664191153</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <f>Sheet1!F65</f>
         <v>6.1026800129157248</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <f>Sheet1!G65</f>
         <v>6.6838876331934136</v>
       </c>
-      <c r="M29">
+      <c r="N29">
+        <v>6.0058120762027771</v>
+      </c>
+      <c r="O29">
         <f>Sheet1!I29</f>
         <v>30.97</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="P29">
+        <v>23348</v>
+      </c>
+      <c r="Q29">
+        <v>2.98</v>
+      </c>
+      <c r="R29">
+        <v>-9</v>
+      </c>
+      <c r="S29">
+        <v>-2</v>
+      </c>
+      <c r="T29">
+        <v>-5</v>
+      </c>
+      <c r="U29">
+        <v>-38</v>
+      </c>
+      <c r="V29">
+        <v>-14</v>
+      </c>
+      <c r="W29" s="3">
+        <v>-13.6</v>
+      </c>
+      <c r="X29">
+        <v>5.1693099785774717</v>
+      </c>
+      <c r="Y29">
+        <v>4.92</v>
+      </c>
+      <c r="Z29">
+        <v>-0.06</v>
+      </c>
+      <c r="AA29">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2102,31 +3387,73 @@
         <v>782</v>
       </c>
       <c r="H30">
+        <v>360</v>
+      </c>
+      <c r="I30">
         <f>Sheet1!C66</f>
         <v>0.10886921178690666</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f>Sheet1!D66</f>
         <v>2.2499637102627377</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f>Sheet1!E66</f>
         <v>8.8546958920017413</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <f>Sheet1!F66</f>
         <v>13.173174626215706</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <f>Sheet1!G66</f>
         <v>28.378574539120336</v>
       </c>
-      <c r="M30">
+      <c r="N30">
+        <v>13.0643054144288</v>
+      </c>
+      <c r="O30">
         <f>Sheet1!I30</f>
         <v>27.556000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="P30">
+        <v>34454</v>
+      </c>
+      <c r="Q30">
+        <v>3.17</v>
+      </c>
+      <c r="R30">
+        <v>-12</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>-15</v>
+      </c>
+      <c r="U30">
+        <v>-35</v>
+      </c>
+      <c r="V30">
+        <v>-14</v>
+      </c>
+      <c r="W30" s="3">
+        <v>-15</v>
+      </c>
+      <c r="X30">
+        <v>6.848867854744638</v>
+      </c>
+      <c r="Y30">
+        <v>4.37</v>
+      </c>
+      <c r="Z30">
+        <v>-2.39</v>
+      </c>
+      <c r="AA30">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2154,31 +3481,73 @@
         <v>2580</v>
       </c>
       <c r="H31">
+        <v>1107</v>
+      </c>
+      <c r="I31">
         <f>Sheet1!C67</f>
         <v>7.9088895919012969E-2</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f>Sheet1!D67</f>
         <v>1.7795001581777918</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f>Sheet1!E67</f>
         <v>13.405567858272699</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <f>Sheet1!F67</f>
         <v>43.854792787092691</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <f>Sheet1!G67</f>
         <v>102.02467573552673</v>
       </c>
-      <c r="M31">
+      <c r="N31">
+        <v>43.775703891173677</v>
+      </c>
+      <c r="O31">
         <f>Sheet1!I31</f>
         <v>25.288</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="P31">
+        <v>29557</v>
+      </c>
+      <c r="Q31">
+        <v>5.57</v>
+      </c>
+      <c r="R31">
+        <v>-30</v>
+      </c>
+      <c r="S31">
+        <v>-9</v>
+      </c>
+      <c r="T31">
+        <v>-20</v>
+      </c>
+      <c r="U31">
+        <v>-40</v>
+      </c>
+      <c r="V31">
+        <v>-24</v>
+      </c>
+      <c r="W31" s="3">
+        <v>-24.6</v>
+      </c>
+      <c r="X31">
+        <v>13.106515506803095</v>
+      </c>
+      <c r="Y31">
+        <v>4.28</v>
+      </c>
+      <c r="Z31">
+        <v>-3.89</v>
+      </c>
+      <c r="AA31">
+        <v>-3.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2206,31 +3575,73 @@
         <v>948</v>
       </c>
       <c r="H32">
+        <v>718</v>
+      </c>
+      <c r="I32">
         <f>Sheet1!C68</f>
         <v>0.14548628791736379</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <f>Sheet1!D68</f>
         <v>2.6914963264712299</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <f>Sheet1!E68</f>
         <v>10.311340656143159</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <f>Sheet1!F68</f>
         <v>13.202880628500765</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <f>Sheet1!G68</f>
         <v>17.240125118207608</v>
       </c>
-      <c r="M32">
+      <c r="N32">
+        <v>13.0573943405834</v>
+      </c>
+      <c r="O32">
         <f>Sheet1!I32</f>
         <v>54.988</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="P32">
+        <v>39411</v>
+      </c>
+      <c r="Q32">
+        <v>5.22</v>
+      </c>
+      <c r="R32">
+        <v>-7</v>
+      </c>
+      <c r="S32">
+        <v>6</v>
+      </c>
+      <c r="T32">
+        <v>-2</v>
+      </c>
+      <c r="U32">
+        <v>-31</v>
+      </c>
+      <c r="V32">
+        <v>-22</v>
+      </c>
+      <c r="W32" s="3">
+        <v>-11.2</v>
+      </c>
+      <c r="X32">
+        <v>15.535464856330181</v>
+      </c>
+      <c r="Y32">
+        <v>3.9</v>
+      </c>
+      <c r="Z32">
+        <v>-4.91</v>
+      </c>
+      <c r="AA32">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2258,31 +3669,73 @@
         <v>3417</v>
       </c>
       <c r="H33">
+        <v>2044</v>
+      </c>
+      <c r="I33">
         <f>Sheet1!C69</f>
         <v>5.8357357112011107E-2</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <f>Sheet1!D69</f>
         <v>1.7507207133603333</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <f>Sheet1!E69</f>
         <v>11.461384936798982</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <f>Sheet1!F69</f>
         <v>23.914844944502153</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f>Sheet1!G69</f>
         <v>39.881417850348392</v>
       </c>
-      <c r="M33">
+      <c r="N33">
+        <v>23.856487587390141</v>
+      </c>
+      <c r="O33">
         <f>Sheet1!I33</f>
         <v>85.679000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="P33">
+        <v>56867</v>
+      </c>
+      <c r="Q33">
+        <v>3.86</v>
+      </c>
+      <c r="R33">
+        <v>-13</v>
+      </c>
+      <c r="S33">
+        <v>-2</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>-41</v>
+      </c>
+      <c r="V33">
+        <v>-22</v>
+      </c>
+      <c r="W33" s="3">
+        <v>-15.4</v>
+      </c>
+      <c r="X33">
+        <v>4.4753519631805041</v>
+      </c>
+      <c r="Y33">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="Z33">
+        <v>-1.37</v>
+      </c>
+      <c r="AA33">
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2310,31 +3763,73 @@
         <v>3931</v>
       </c>
       <c r="H34">
+        <v>1532</v>
+      </c>
+      <c r="I34">
         <f>Sheet1!C70</f>
         <v>0.1292209337912742</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <f>Sheet1!D70</f>
         <v>0.79572890808310948</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f>Sheet1!E70</f>
         <v>2.781650627401639</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <f>Sheet1!F70</f>
         <v>10.548508858435067</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <f>Sheet1!G70</f>
         <v>26.735131091236781</v>
       </c>
-      <c r="M34">
+      <c r="N34">
+        <v>10.419287924643793</v>
+      </c>
+      <c r="O34">
         <f>Sheet1!I34</f>
         <v>147.035</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="P34">
+        <v>108407</v>
+      </c>
+      <c r="Q34">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="R34">
+        <v>-19</v>
+      </c>
+      <c r="S34">
+        <v>-7</v>
+      </c>
+      <c r="T34">
+        <v>-16</v>
+      </c>
+      <c r="U34">
+        <v>-36</v>
+      </c>
+      <c r="V34">
+        <v>-22</v>
+      </c>
+      <c r="W34" s="3">
+        <v>-20</v>
+      </c>
+      <c r="X34">
+        <v>8.6667385815639122</v>
+      </c>
+      <c r="Y34">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="Z34">
+        <v>-2.37</v>
+      </c>
+      <c r="AA34">
+        <v>-4.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2362,28 +3857,70 @@
         <v>674</v>
       </c>
       <c r="H35">
+        <v>290</v>
+      </c>
+      <c r="I35">
         <f>Sheet1!C71</f>
         <v>0.5924323210468021</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <f>Sheet1!D71</f>
         <v>2.447003065193313</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f>Sheet1!E71</f>
         <v>6.0788707724802311</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <f>Sheet1!F71</f>
         <v>8.0622311516369169</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <f>Sheet1!G71</f>
         <v>17.360842799371508</v>
       </c>
-      <c r="M35">
+      <c r="N35">
+        <v>7.4697988305901148</v>
+      </c>
+      <c r="O35">
         <f>Sheet1!I35</f>
         <v>38.823</v>
+      </c>
+      <c r="P35">
+        <v>34728</v>
+      </c>
+      <c r="Q35">
+        <v>3.38</v>
+      </c>
+      <c r="R35">
+        <v>-24</v>
+      </c>
+      <c r="S35">
+        <v>-17</v>
+      </c>
+      <c r="T35">
+        <v>-34</v>
+      </c>
+      <c r="U35">
+        <v>-57</v>
+      </c>
+      <c r="V35">
+        <v>-32</v>
+      </c>
+      <c r="W35" s="3">
+        <v>-32.799999999999997</v>
+      </c>
+      <c r="X35">
+        <v>18.970781542641252</v>
+      </c>
+      <c r="Y35">
+        <v>-0.17</v>
+      </c>
+      <c r="Z35">
+        <v>-6.74</v>
+      </c>
+      <c r="AA35">
+        <v>-6.65</v>
       </c>
     </row>
   </sheetData>
@@ -2397,10 +3934,10 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>